<commit_message>
docs: integrate chart for run time vs actions
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janma\Documents\JM\Unecrypted\Udacity - Data Science\AI Nanodegree\Project 2\My Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE0A000-2CF7-4FB6-BF3C-91CB1A78F9D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D92C9A-B7D7-4011-B45B-69613827A3E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -287,15 +287,6 @@
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -303,15 +294,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -337,6 +319,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,6 +352,1794 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="cs-CZ"/>
+              <a:t>Run time per algorithm</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>breadth first search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$C$4,List1!$C$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$C$9,List1!$C$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.9037999997854002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1829658000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F005-4B1D-8E8F-F3317EF1D7E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>depth first search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$D$4,List1!$D$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$D$9,List1!$D$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.5582000000904301E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5887878000012201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F005-4B1D-8E8F-F3317EF1D7E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>uniform cost search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$E$4,List1!$E$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$E$9,List1!$E$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4.5175000000199301E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7790035999996601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F005-4B1D-8E8F-F3317EF1D7E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greedy best first search
+ - h_pg_levelsum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$G$4,List1!$G$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$G$9,List1!$G$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.250989199999821</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.84972709999965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F005-4B1D-8E8F-F3317EF1D7E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greedy best first search
+ - h_pg_maxlevel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$H$4,List1!$H$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$H$9,List1!$H$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.17961519999971601</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.688836799999899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-F005-4B1D-8E8F-F3317EF1D7E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greedy best first search
+ - h_pg_maxlevel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$H$4,List1!$H$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$H$9,List1!$H$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.17961519999971601</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.688836799999899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-F005-4B1D-8E8F-F3317EF1D7E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greedy best first search
+ - h_pg_setlevel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$I$4,List1!$I$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$I$9,List1!$I$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.38819860000012302</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.2970900000000203</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-F005-4B1D-8E8F-F3317EF1D7E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a* search
+ - h_unmet_goals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$J$4,List1!$J$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$J$9,List1!$J$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5.0629000002118101E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3056961000002001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-F005-4B1D-8E8F-F3317EF1D7E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a* search
+ - h_pg_maxlevel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$L$4,List1!$L$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$L$9,List1!$L$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.63218820000020004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1115.4357104999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-F005-4B1D-8E8F-F3317EF1D7E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$M$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a* search
+ - h_pg_setlevel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$M$4,List1!$M$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$M$9,List1!$M$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.82654090000005398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>993.091442999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-F005-4B1D-8E8F-F3317EF1D7E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2032112287"/>
+        <c:axId val="1901876015"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2032112287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Actions</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1901876015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1901876015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Run</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="cs-CZ" baseline="0"/>
+                  <a:t> Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2032112287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{184AED4C-29DB-4609-9467-C5858CD63A14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -619,8 +2407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,533 +2429,533 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="3"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="21"/>
     </row>
     <row r="3" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="10">
         <v>20</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="10">
         <v>20</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="10">
         <v>20</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="10">
         <v>20</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="10">
         <v>20</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="10">
         <v>20</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="10">
         <v>20</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="10">
         <v>20</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="10">
         <v>20</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="10">
         <v>20</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="11">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="12">
         <v>43</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="12">
         <v>21</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="12">
         <v>60</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="12">
         <v>7</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="12">
         <v>6</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="12">
         <v>6</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="12">
         <v>6</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="12">
         <v>50</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="12">
         <v>28</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="12">
         <v>43</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="13">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="23"/>
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="12">
         <v>56</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="12">
         <v>22</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="12">
         <v>62</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="12">
         <v>9</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="12">
         <v>8</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="12">
         <v>8</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="12">
         <v>8</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="12">
         <v>52</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="12">
         <v>30</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="12">
         <v>45</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="13">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="12">
         <v>178</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="12">
         <v>84</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="12">
         <v>240</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="12">
         <v>29</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="12">
         <v>28</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="12">
         <v>24</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="12">
         <v>28</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="12">
         <v>206</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="12">
         <v>122</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="12">
         <v>180</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="13">
         <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="23"/>
+      <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="15">
         <v>6</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="15">
         <v>6</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="15">
         <v>6</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="15">
         <v>6</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="15">
         <v>6</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="15">
         <v>6</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="15">
         <v>6</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="15">
         <v>6</v>
       </c>
-      <c r="K8" s="21">
+      <c r="K8" s="15">
         <v>6</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="15">
         <v>6</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <v>2.9037999997854002E-3</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="2">
         <v>1.5582000000904301E-3</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="2">
         <v>4.5175000000199301E-3</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="2">
         <v>1.6421000000264E-3</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="2">
         <v>0.250989199999821</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="2">
         <v>0.17961519999971601</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="2">
         <v>0.38819860000012302</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="2">
         <v>5.0629000002118101E-3</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="2">
         <v>0.68454999999994404</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="2">
         <v>0.63218820000020004</v>
       </c>
-      <c r="M9" s="20">
+      <c r="M9" s="14">
         <v>0.82654090000005398</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="10">
         <v>72</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="16">
         <v>72</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="10">
         <v>72</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="10">
         <v>72</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="10">
         <v>72</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="10">
         <v>72</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="10">
         <v>72</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10" s="10">
         <v>72</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="10">
         <v>72</v>
       </c>
-      <c r="L10" s="16">
+      <c r="L10" s="10">
         <v>72</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="11">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="12">
         <v>3343</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="15">
         <v>624</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="12">
         <v>5154</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="12">
         <v>17</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="12">
         <v>9</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="12">
         <v>27</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="15">
         <v>9</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="15">
         <v>2467</v>
       </c>
-      <c r="K11" s="21">
+      <c r="K11" s="15">
         <v>357</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="15">
         <v>2887</v>
       </c>
-      <c r="M11" s="19">
+      <c r="M11" s="13">
         <v>1037</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="23"/>
+      <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="12">
         <v>4609</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="15">
         <v>625</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="12">
         <v>5156</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="12">
         <v>19</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="12">
         <v>11</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="12">
         <v>29</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="15">
         <v>11</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="15">
         <v>2469</v>
       </c>
-      <c r="K12" s="21">
+      <c r="K12" s="15">
         <v>359</v>
       </c>
-      <c r="L12" s="21">
+      <c r="L12" s="15">
         <v>2889</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="13">
         <v>1039</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="12">
         <v>30503</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="15">
         <v>5602</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="12">
         <v>46618</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="12">
         <v>170</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="12">
         <v>86</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="12">
         <v>249</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="15">
         <v>84</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="15">
         <v>22522</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="15">
         <v>3426</v>
       </c>
-      <c r="L13" s="21">
+      <c r="L13" s="15">
         <v>26594</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13" s="13">
         <v>9605</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="12" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="12">
         <v>9</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="15">
         <v>619</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="12">
         <v>9</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="12">
         <v>9</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="12">
         <v>9</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="12">
         <v>9</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="15">
         <v>9</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="15">
         <v>9</v>
       </c>
-      <c r="K14" s="21">
+      <c r="K14" s="15">
         <v>9</v>
       </c>
-      <c r="L14" s="21">
+      <c r="L14" s="15">
         <v>9</v>
       </c>
-      <c r="M14" s="19">
+      <c r="M14" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="13" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="2">
         <v>1.1829658000006</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="17">
         <v>1.5887878000012201</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="2">
         <v>1.7790035999996601</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="2">
         <v>1.3352000000850199E-2</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="2">
         <v>5.84972709999965</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="2">
         <v>11.688836799999899</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="2">
         <v>9.2970900000000203</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="2">
         <v>1.3056961000002001</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="2">
         <v>183.37924109999901</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="2">
         <v>1115.4357104999999</v>
       </c>
-      <c r="M15" s="20">
+      <c r="M15" s="14">
         <v>993.091442999999</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="D16" s="24"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="D16" s="18"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1187,5 +2975,6 @@
     <mergeCell ref="A10:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: integrate chart for expansions vs actions
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janma\Documents\JM\Unecrypted\Udacity - Data Science\AI Nanodegree\Project 2\My Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D92C9A-B7D7-4011-B45B-69613827A3E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C587413-AA68-44E4-9E64-D05AD6B7B037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1545,6 +1545,1193 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="cs-CZ"/>
+              <a:t>Expansions per algorithm</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>breadth first search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$C$4,List1!$C$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$C$5,List1!$C$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3343</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4864-4296-8468-F423A979E236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>depth first search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$D$4,List1!$D$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$E$5,List1!$E$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4864-4296-8468-F423A979E236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>uniform cost search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$E$4,List1!$E$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$E$5,List1!$E$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4864-4296-8468-F423A979E236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greedy best first search
+ - h_pg_levelsum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$G$4,List1!$G$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$F$5,List1!$F$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4864-4296-8468-F423A979E236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greedy best first search
+ - h_pg_maxlevel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$H$4,List1!$H$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$H$5,List1!$H$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4864-4296-8468-F423A979E236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greedy best first search
+ - h_pg_maxlevel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$H$4,List1!$H$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$H$5,List1!$H$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-4864-4296-8468-F423A979E236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greedy best first search
+ - h_pg_setlevel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$I$4,List1!$I$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$I$5,List1!$I$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4864-4296-8468-F423A979E236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a* search
+ - h_unmet_goals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$J$4,List1!$J$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$J$5,List1!$J$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2467</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-4864-4296-8468-F423A979E236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a* search
+ - h_pg_maxlevel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$L$4,List1!$L$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$L$5,List1!$L$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2887</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-4864-4296-8468-F423A979E236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$M$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a* search
+ - h_pg_setlevel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(List1!$M$4,List1!$M$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(List1!$M$5,List1!$M$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1037</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-4864-4296-8468-F423A979E236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2032112287"/>
+        <c:axId val="1901876015"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2032112287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Actions</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1901876015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1901876015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Expansions</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2032112287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1585,7 +2772,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2134,6 +3877,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1485900</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2B1758C-BD92-4168-B8F8-BD8745D2C64B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2407,8 +4188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>